<commit_message>
Added sample, fixed some syntax highlighting.
</commit_message>
<xml_diff>
--- a/src/ConnectQl.Sample.NetCore/Example.xlsx
+++ b/src/ConnectQl.Sample.NetCore/Example.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>first</t>
   </si>
@@ -21,6 +21,9 @@
   </si>
   <si>
     <t>third</t>
+  </si>
+  <si>
+    <t>fourth</t>
   </si>
   <si>
     <t>three</t>
@@ -76,7 +79,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -85,6 +88,7 @@
     <col min="1" max="1" width="9.140625" customWidth="1"/>
     <col min="2" max="2" width="9.140625" customWidth="1"/>
     <col min="3" max="3" width="9.140625" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -97,6 +101,9 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
@@ -106,7 +113,12 @@
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="D3" s="0" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>